<commit_message>
Updated (final) version of the it admin board
</commit_message>
<xml_diff>
--- a/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
+++ b/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyanova\Documents\GitHub\peakboard-templates.github.io\_templates\IT-Admin-Ticket-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F2598-F9AE-4266-83F5-2494A44C03EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7624FE9C-B3E0-4D80-AC66-8E105B0380EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Tickets" sheetId="1" r:id="rId1"/>
-    <sheet name="Tickets" sheetId="2" r:id="rId2"/>
-    <sheet name="Solved tickets in a year" sheetId="3" r:id="rId3"/>
+    <sheet name="Solved tickets in a year" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,91 +31,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ticket</t>
   </si>
   <si>
-    <t xml:space="preserve">High </t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Connection impossible</t>
-  </si>
-  <si>
     <t>API not provided</t>
   </si>
   <si>
     <t>Box not working</t>
   </si>
   <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Amount solved tickets</t>
-  </si>
-  <si>
-    <t>Amount all tickets</t>
-  </si>
-  <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>Function not working</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Cannot connect to the box</t>
+  </si>
+  <si>
+    <t>Cannot update the designer</t>
+  </si>
+  <si>
+    <t>Cable missing</t>
+  </si>
+  <si>
+    <t>Box too hot</t>
+  </si>
+  <si>
+    <t>Cannot install designer</t>
+  </si>
+  <si>
+    <t>amount_closed_tickets</t>
+  </si>
+  <si>
+    <t>amount_all_tickets</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,13 +118,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,59 +441,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
+      <c r="B6">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -522,202 +531,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B4822-D87C-4C70-9C75-2C32C2627802}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>80</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <f>A2-B2</f>
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11F88D6-7E73-45D2-BCE2-0BB41D2F6FE2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43739</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
       <c r="C2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B3">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C6">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B7">
         <v>50</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B8">
         <v>70</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B9">
         <v>40</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B10">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B13">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>80</v>
-      </c>
-      <c r="C12">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DE and EN version of the IT Admin Board done
</commit_message>
<xml_diff>
--- a/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
+++ b/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
@@ -1,40 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyanova\Documents\GitHub\peakboard-templates.github.io\_templates\IT-Admin-Ticket-Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimi\Desktop\Zusatz\Arbeit\Peakboard\peakboard-templates.github.io\_templates\IT-Admin-Ticket-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7624FE9C-B3E0-4D80-AC66-8E105B0380EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21C5301-056B-4014-8BA5-A8672A1AC1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Tickets" sheetId="1" r:id="rId1"/>
     <sheet name="Solved tickets in a year" sheetId="3" r:id="rId2"/>
+    <sheet name="Offene Tickets" sheetId="4" r:id="rId3"/>
+    <sheet name="Geschlossene Tickets pro Jahr" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Ticket</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>API not provided</t>
   </si>
@@ -45,9 +34,6 @@
     <t>Function not working</t>
   </si>
   <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Cannot connect to the box</t>
   </si>
   <si>
@@ -70,6 +56,36 @@
   </si>
   <si>
     <t>month</t>
+  </si>
+  <si>
+    <t>Keine Verbindung zur Box</t>
+  </si>
+  <si>
+    <t>Keine API zur Verfügung gestellt</t>
+  </si>
+  <si>
+    <t>Box funktioniert nicht</t>
+  </si>
+  <si>
+    <t>Funktion fehlt</t>
+  </si>
+  <si>
+    <t>Designer kann nicht aktualisiert werden</t>
+  </si>
+  <si>
+    <t>Kabel fehlt</t>
+  </si>
+  <si>
+    <t>Box zu heiß</t>
+  </si>
+  <si>
+    <t>Designer kann nicht installiert werden</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -77,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -120,7 +136,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -444,82 +460,82 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>120</v>
@@ -534,27 +550,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11F88D6-7E73-45D2-BCE2-0BB41D2F6FE2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43739</v>
       </c>
@@ -565,7 +583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43770</v>
       </c>
@@ -576,7 +594,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43800</v>
       </c>
@@ -587,7 +605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43831</v>
       </c>
@@ -598,7 +616,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43862</v>
       </c>
@@ -609,7 +627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43891</v>
       </c>
@@ -620,7 +638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43922</v>
       </c>
@@ -631,7 +649,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43952</v>
       </c>
@@ -642,7 +660,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43983</v>
       </c>
@@ -653,7 +671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44013</v>
       </c>
@@ -664,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44044</v>
       </c>
@@ -675,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44075</v>
       </c>
@@ -691,4 +709,249 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D571A962-1E82-4B6A-BE29-E500FB93D7F9}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A262FBA1-06CD-4B51-BDB7-7ADC8765A909}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>43739</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B3">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DE and EN version edited
</commit_message>
<xml_diff>
--- a/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
+++ b/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimi\Desktop\Zusatz\Arbeit\Peakboard\peakboard-templates.github.io\_templates\IT-Admin-Ticket-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21C5301-056B-4014-8BA5-A8672A1AC1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F1BD93-CC96-4B0B-B71D-16618BEDBE29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Tickets" sheetId="1" r:id="rId1"/>
     <sheet name="Solved tickets in a year" sheetId="3" r:id="rId2"/>
     <sheet name="Offene Tickets" sheetId="4" r:id="rId3"/>
-    <sheet name="Geschlossene Tickets pro Jahr" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>API not provided</t>
   </si>
@@ -86,6 +85,72 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>Verbindung per ODBC fehlgeschlagen</t>
+  </si>
+  <si>
+    <t>Allgemeine technische Frage</t>
+  </si>
+  <si>
+    <t>Keine SAP Daten</t>
+  </si>
+  <si>
+    <t>Fehler beim Editieren einer Variable</t>
+  </si>
+  <si>
+    <t>Scripting Problem</t>
+  </si>
+  <si>
+    <t>Probleme mit dem Bearbeiten von Schriftarten</t>
+  </si>
+  <si>
+    <t>Authentifizierung mit JSON nicht möglich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download Fehler </t>
+  </si>
+  <si>
+    <t>Sonderzeichen im Passwort nicht akzeptiert</t>
+  </si>
+  <si>
+    <t>Fehlermeldung</t>
+  </si>
+  <si>
+    <t>Databinding Listview not working</t>
+  </si>
+  <si>
+    <t>SQL Async</t>
+  </si>
+  <si>
+    <t>Connection via ODBC failed</t>
+  </si>
+  <si>
+    <t>General technical question</t>
+  </si>
+  <si>
+    <t>Error editing a variable</t>
+  </si>
+  <si>
+    <t>No SAP data</t>
+  </si>
+  <si>
+    <t>Problems with editing fonts</t>
+  </si>
+  <si>
+    <t>Authentication with JSON not possible</t>
+  </si>
+  <si>
+    <t>Download error</t>
+  </si>
+  <si>
+    <t>Special characters in password not accepted</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>Databinding Listview funktioniert nicht</t>
   </si>
 </sst>
 </file>
@@ -457,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,6 +606,102 @@
         <v>120</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -548,10 +709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11F88D6-7E73-45D2-BCE2-0BB41D2F6FE2}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,10 +738,10 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C2">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -588,10 +749,10 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="C3">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -599,10 +760,10 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -610,10 +771,10 @@
         <v>43831</v>
       </c>
       <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
         <v>40</v>
-      </c>
-      <c r="C5">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -621,10 +782,10 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -632,10 +793,10 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -643,10 +804,10 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C8">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -657,7 +818,7 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -665,10 +826,10 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -676,10 +837,10 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -687,10 +848,10 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -698,10 +859,87 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B17">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -713,13 +951,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D571A962-1E82-4B6A-BE29-E500FB93D7F9}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -793,162 +1034,100 @@
         <v>120</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A262FBA1-06CD-4B51-BDB7-7ADC8765A909}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>43739</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43770</v>
-      </c>
-      <c r="B3">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>43800</v>
-      </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>43862</v>
-      </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43891</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>43922</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>43952</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-      <c r="C9">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>43983</v>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>44013</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>44044</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>44075</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
+      <c r="B14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated screenshots, inital readme files, updated german version
</commit_message>
<xml_diff>
--- a/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
+++ b/_templates/IT-Admin-Ticket-Board/IT-Tickets.xlsx
@@ -1,62 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimi\Desktop\Zusatz\Arbeit\Peakboard\peakboard-templates.github.io\_templates\IT-Admin-Ticket-Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/IT-Admin-Ticket-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8671E3D-B4A0-4D2E-A477-41A2B75ECA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6834ED1F-FE8A-9C41-AA1C-1809617E9E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30160" windowHeight="18920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Open Tickets" sheetId="1" r:id="rId1"/>
-    <sheet name="Solved tickets in a year" sheetId="3" r:id="rId2"/>
+    <sheet name="Solved tickets in a year" sheetId="3" r:id="rId1"/>
+    <sheet name="Open Tickets" sheetId="1" r:id="rId2"/>
     <sheet name="Offene Tickets" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
-    <t>API not provided</t>
-  </si>
-  <si>
-    <t>Cable missing</t>
-  </si>
-  <si>
-    <t>amount_closed_tickets</t>
-  </si>
-  <si>
-    <t>amount_all_tickets</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
-    <t>Keine API zur Verfügung gestellt</t>
-  </si>
-  <si>
-    <t>Funktion fehlt</t>
-  </si>
-  <si>
-    <t>Kabel fehlt</t>
-  </si>
-  <si>
     <t>ticket</t>
   </si>
   <si>
     <t>priority</t>
   </si>
   <si>
-    <t>Allgemeine technische Frage</t>
-  </si>
-  <si>
     <t>Scripting Problem</t>
   </si>
   <si>
@@ -87,27 +73,15 @@
     <t>Error message</t>
   </si>
   <si>
-    <t>amount_open_tickets</t>
-  </si>
-  <si>
     <t>Cannot connect to wi-fi</t>
   </si>
   <si>
-    <t>Router not working</t>
-  </si>
-  <si>
     <t>Laptop keyboard not working</t>
   </si>
   <si>
     <t>Cannot update Windows</t>
   </si>
   <si>
-    <t>PC too hot</t>
-  </si>
-  <si>
-    <t>Cannot install the software</t>
-  </si>
-  <si>
     <t>Connection via LAN cable failed</t>
   </si>
   <si>
@@ -120,27 +94,15 @@
     <t>Laptop cannot be charged</t>
   </si>
   <si>
-    <t>Keine Verbindung zur WLAN</t>
-  </si>
-  <si>
     <t>Router funktioniert nicht</t>
   </si>
   <si>
     <t>Windows kann nicht aktualisiert werden</t>
   </si>
   <si>
-    <t>PC zu heiß</t>
-  </si>
-  <si>
     <t>Software kann nicht installiert werden</t>
   </si>
   <si>
-    <t>Verbindung per LAN Kabel fehlgeschlagen</t>
-  </si>
-  <si>
-    <t>Fehler beim Desktopeinstellen</t>
-  </si>
-  <si>
     <t>Network problem</t>
   </si>
   <si>
@@ -157,6 +119,54 @@
   </si>
   <si>
     <t>Laptop kann nicht aufgeladen werden</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>WLAN im 4. Stock funktioniert nicht</t>
+  </si>
+  <si>
+    <t>HDMI Kabel im Besprechungsraum 5 defekt</t>
+  </si>
+  <si>
+    <t>PC wird zu heiß</t>
+  </si>
+  <si>
+    <t>API steht nicht mehr zur Verfügung</t>
+  </si>
+  <si>
+    <t>Neues CRM aufsetzen</t>
+  </si>
+  <si>
+    <t>Fehler beim Desktop einstellen</t>
+  </si>
+  <si>
+    <t>Passwort zurücksetzen funktioniert nicht</t>
+  </si>
+  <si>
+    <t>WLAN Drucker in Gang 6 defekt</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Rest API doesn't work anymore</t>
+  </si>
+  <si>
+    <t>Router not working on 6th floor</t>
+  </si>
+  <si>
+    <t>Missing HDMI cable in conference room 6</t>
+  </si>
+  <si>
+    <t>PC gets too hot</t>
+  </si>
+  <si>
+    <t>Cannot install new ERP software</t>
   </si>
 </sst>
 </file>
@@ -164,7 +174,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -207,7 +217,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -215,8 +225,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -232,7 +242,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -527,223 +537,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11F88D6-7E73-45D2-BCE2-0BB41D2F6FE2}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43739</v>
       </c>
@@ -754,41 +577,41 @@
         <v>92</v>
       </c>
       <c r="D2">
-        <f>C2-B2</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>42+(C2-B2)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>108</v>
       </c>
       <c r="D3">
         <f>D2+(C3-B3)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D20" si="0">D3+(C4-B4)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43831</v>
       </c>
@@ -800,40 +623,40 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>54</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43922</v>
       </c>
@@ -845,10 +668,10 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43952</v>
       </c>
@@ -860,10 +683,10 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43983</v>
       </c>
@@ -875,10 +698,10 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44013</v>
       </c>
@@ -886,44 +709,44 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>20</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44105</v>
       </c>
@@ -935,25 +758,25 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C15">
         <v>56</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44166</v>
       </c>
@@ -965,10 +788,10 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44197</v>
       </c>
@@ -980,10 +803,10 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44228</v>
       </c>
@@ -995,37 +818,37 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>25</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>24</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>141</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1035,182 +858,369 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D571A962-1E82-4B6A-BE29-E500FB93D7F9}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>100</v>

</xml_diff>